<commit_message>
Added a simple JS example. Fixed min json formats.
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-strings.xlsx
+++ b/examples/test-js/dink-content/main-strings.xlsx
@@ -40,6 +40,18 @@
     <x:t/>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Part1_VXIU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Part2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>scene1_Scene1_Part2_CF6W</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Part3</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Part3_9MXL</x:t>
   </x:si>
   <x:si>
@@ -49,6 +61,12 @@
     <x:t>DAVE</x:t>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Part3_YTMH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Part4</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Part4_T9GZ</x:t>
   </x:si>
   <x:si>
@@ -94,36 +112,87 @@
     <x:t>GEORGE</x:t>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Part4_PZV1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Back</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
   </x:si>
   <x:si>
     <x:t>You sure you want to go right?</x:t>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Right_P8FP</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
   </x:si>
   <x:si>
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Left_WXCN</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_OtherContent_FSDK</x:t>
   </x:si>
   <x:si>
     <x:t>This content is nothing at all to do with Dink!</x:t>
   </x:si>
   <x:si>
+    <x:t>scene1_OtherContent_VZWQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_QU2R</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barks</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_X20S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Intro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_OQ5O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Intro2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_NEAB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TestScene</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_AD94</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Scene1</x:t>
+  </x:si>
+  <x:si>
     <x:t>main_Intro_FDAP</x:t>
   </x:si>
   <x:si>
     <x:t>This is a test file.</x:t>
   </x:si>
   <x:si>
+    <x:t>main_Intro_EBU9</x:t>
+  </x:si>
+  <x:si>
     <x:t>main_Intro2_PCBU</x:t>
   </x:si>
   <x:si>
     <x:t>LAURA: This is an earlier line I am saying.</x:t>
   </x:si>
   <x:si>
+    <x:t>main_Intro2_QEUQ</x:t>
+  </x:si>
+  <x:si>
     <x:t>main_TestScene_16U4</x:t>
   </x:si>
   <x:si>
@@ -154,6 +223,9 @@
     <x:t>Glad that's over with!</x:t>
   </x:si>
   <x:si>
+    <x:t>main_TestScene_MP0B</x:t>
+  </x:si>
+  <x:si>
     <x:t>main_Barks_O037</x:t>
   </x:si>
   <x:si>
@@ -197,6 +269,9 @@
   </x:si>
   <x:si>
     <x:t>Bark6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_83WH</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -280,8 +355,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D26" totalsRowShown="0">
-  <x:autoFilter ref="A1:D26"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D42" totalsRowShown="0">
+  <x:autoFilter ref="A1:D42"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="ID"/>
     <x:tableColumn id="2" name="Text"/>
@@ -580,7 +655,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D26"/>
+  <x:dimension ref="A1:D42"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -628,7 +703,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>7</x:v>
@@ -636,10 +711,10 @@
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>12</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>7</x:v>
@@ -650,13 +725,13 @@
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="A5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>6</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>7</x:v>
@@ -684,7 +759,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>7</x:v>
@@ -698,7 +773,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>7</x:v>
@@ -712,7 +787,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>7</x:v>
@@ -726,7 +801,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>7</x:v>
@@ -734,13 +809,13 @@
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="A11" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>7</x:v>
@@ -748,13 +823,13 @@
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="A12" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>7</x:v>
@@ -762,13 +837,13 @@
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="A13" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="B13" s="0" t="s">
+      <x:c r="C13" s="0" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>7</x:v>
@@ -796,7 +871,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>7</x:v>
@@ -807,10 +882,10 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
         <x:v>7</x:v>
@@ -818,27 +893,27 @@
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>7</x:v>
@@ -846,13 +921,13 @@
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>7</x:v>
@@ -860,13 +935,13 @@
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>7</x:v>
@@ -874,13 +949,13 @@
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
         <x:v>7</x:v>
@@ -888,13 +963,13 @@
     </x:row>
     <x:row r="22" spans="1:4">
       <x:c r="A22" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
         <x:v>7</x:v>
@@ -902,13 +977,13 @@
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="A23" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>7</x:v>
@@ -916,13 +991,13 @@
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="A24" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
         <x:v>7</x:v>
@@ -930,13 +1005,13 @@
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="A25" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
         <x:v>7</x:v>
@@ -944,15 +1019,239 @@
     </x:row>
     <x:row r="26" spans="1:4">
       <x:c r="A26" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="B26" s="0" t="s">
+      <x:c r="B30" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="C26" s="0" t="s">
+      <x:c r="C30" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="A31" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="A32" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D26" s="0" t="s">
+      <x:c r="D32" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="A33" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="A34" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="A35" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4">
+      <x:c r="A36" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="A37" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="A38" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4">
+      <x:c r="A39" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="A40" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="A41" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4">
+      <x:c r="A42" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>

</xml_diff>